<commit_message>
Changes to some of the plot chunks - error fixes
</commit_message>
<xml_diff>
--- a/aapl.xlsx
+++ b/aapl.xlsx
@@ -1,75 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/286054357d240948/Github/Intro to Finance/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_8FE7FFC08F79A8536E3CA493EA7BD272EAC5DFEF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4005B937-B49F-4170-8E70-70092204C523}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="1920" windowWidth="21600" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="9">
-  <si>
-    <t>symbol</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>close</t>
-  </si>
-  <si>
-    <t>volume</t>
-  </si>
-  <si>
-    <t>adjusted</t>
-  </si>
-  <si>
-    <t>AAPL</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd HH:mm:ss UTC"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,14 +67,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -172,7 +113,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -204,27 +145,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -256,24 +179,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -449,58 +354,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>close</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>volume</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>adjusted</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B2" s="2">
         <v>44886</v>
       </c>
       <c r="C2">
-        <v>150.16000399999999</v>
+        <v>150.160004</v>
       </c>
       <c r="D2">
-        <v>150.36999499999999</v>
+        <v>150.369995</v>
       </c>
       <c r="E2">
         <v>147.720001</v>
@@ -515,18 +434,20 @@
         <v>148.009995</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B3" s="2">
         <v>44887</v>
       </c>
       <c r="C3">
-        <v>148.13000500000001</v>
+        <v>148.130005</v>
       </c>
       <c r="D3">
-        <v>150.41999799999999</v>
+        <v>150.419998</v>
       </c>
       <c r="E3">
         <v>146.929993</v>
@@ -541,9 +462,11 @@
         <v>150.179993</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B4" s="2">
         <v>44888</v>
@@ -552,10 +475,10 @@
         <v>149.449997</v>
       </c>
       <c r="D4">
-        <v>151.83000200000001</v>
+        <v>151.830002</v>
       </c>
       <c r="E4">
-        <v>149.33999600000001</v>
+        <v>149.339996</v>
       </c>
       <c r="F4">
         <v>151.070007</v>
@@ -567,47 +490,51 @@
         <v>151.070007</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B5" s="2">
         <v>44890</v>
       </c>
       <c r="C5">
-        <v>148.30999800000001</v>
+        <v>148.309998</v>
       </c>
       <c r="D5">
-        <v>148.88000500000001</v>
+        <v>148.880005</v>
       </c>
       <c r="E5">
-        <v>147.11999499999999</v>
+        <v>147.119995</v>
       </c>
       <c r="F5">
-        <v>148.11000100000001</v>
+        <v>148.110001</v>
       </c>
       <c r="G5">
         <v>35195900</v>
       </c>
       <c r="H5">
-        <v>148.11000100000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
+        <v>148.110001</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B6" s="2">
         <v>44893</v>
       </c>
       <c r="C6">
-        <v>145.13999899999999</v>
+        <v>145.139999</v>
       </c>
       <c r="D6">
-        <v>146.63999899999999</v>
+        <v>146.639999</v>
       </c>
       <c r="E6">
-        <v>143.38000500000001</v>
+        <v>143.380005</v>
       </c>
       <c r="F6">
         <v>144.220001</v>
@@ -619,41 +546,45 @@
         <v>144.220001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B7" s="2">
         <v>44894</v>
       </c>
       <c r="C7">
-        <v>144.28999300000001</v>
+        <v>144.289993</v>
       </c>
       <c r="D7">
-        <v>144.80999800000001</v>
+        <v>144.809998</v>
       </c>
       <c r="E7">
-        <v>140.35000600000001</v>
+        <v>140.350006</v>
       </c>
       <c r="F7">
-        <v>141.16999799999999</v>
+        <v>141.169998</v>
       </c>
       <c r="G7">
         <v>83763800</v>
       </c>
       <c r="H7">
-        <v>141.16999799999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
+        <v>141.169998</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B8" s="2">
         <v>44895</v>
       </c>
       <c r="C8">
-        <v>141.39999399999999</v>
+        <v>141.399994</v>
       </c>
       <c r="D8">
         <v>148.720001</v>
@@ -671,61 +602,67 @@
         <v>148.029999</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B9" s="2">
         <v>44896</v>
       </c>
       <c r="C9">
-        <v>148.21000699999999</v>
+        <v>148.210007</v>
       </c>
       <c r="D9">
-        <v>149.13000500000001</v>
+        <v>149.130005</v>
       </c>
       <c r="E9">
-        <v>146.61000100000001</v>
+        <v>146.610001</v>
       </c>
       <c r="F9">
-        <v>148.30999800000001</v>
+        <v>148.309998</v>
       </c>
       <c r="G9">
         <v>71250400</v>
       </c>
       <c r="H9">
-        <v>148.30999800000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
+        <v>148.309998</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B10" s="2">
         <v>44897</v>
       </c>
       <c r="C10">
-        <v>145.96000699999999</v>
+        <v>145.960007</v>
       </c>
       <c r="D10">
         <v>148</v>
       </c>
       <c r="E10">
-        <v>145.64999399999999</v>
+        <v>145.649994</v>
       </c>
       <c r="F10">
-        <v>147.80999800000001</v>
+        <v>147.809998</v>
       </c>
       <c r="G10">
         <v>65447400</v>
       </c>
       <c r="H10">
-        <v>147.80999800000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
+        <v>147.809998</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B11" s="2">
         <v>44900</v>
@@ -734,24 +671,26 @@
         <v>147.770004</v>
       </c>
       <c r="D11">
-        <v>150.91999799999999</v>
+        <v>150.919998</v>
       </c>
       <c r="E11">
         <v>145.770004</v>
       </c>
       <c r="F11">
-        <v>146.63000500000001</v>
+        <v>146.630005</v>
       </c>
       <c r="G11">
         <v>68826400</v>
       </c>
       <c r="H11">
-        <v>146.63000500000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
+        <v>146.630005</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B12" s="2">
         <v>44901</v>
@@ -763,99 +702,107 @@
         <v>147.300003</v>
       </c>
       <c r="E12">
-        <v>141.91999799999999</v>
+        <v>141.919998</v>
       </c>
       <c r="F12">
-        <v>142.91000399999999</v>
+        <v>142.910004</v>
       </c>
       <c r="G12">
         <v>64727200</v>
       </c>
       <c r="H12">
-        <v>142.91000399999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>8</v>
+        <v>142.910004</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B13" s="2">
         <v>44902</v>
       </c>
       <c r="C13">
-        <v>142.19000199999999</v>
+        <v>142.190002</v>
       </c>
       <c r="D13">
-        <v>143.36999499999999</v>
+        <v>143.369995</v>
       </c>
       <c r="E13">
         <v>140</v>
       </c>
       <c r="F13">
-        <v>140.94000199999999</v>
+        <v>140.940002</v>
       </c>
       <c r="G13">
         <v>69721100</v>
       </c>
       <c r="H13">
-        <v>140.94000199999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>8</v>
+        <v>140.940002</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B14" s="2">
         <v>44903</v>
       </c>
       <c r="C14">
-        <v>142.36000100000001</v>
+        <v>142.360001</v>
       </c>
       <c r="D14">
         <v>143.520004</v>
       </c>
       <c r="E14">
-        <v>141.10000600000001</v>
+        <v>141.100006</v>
       </c>
       <c r="F14">
-        <v>142.64999399999999</v>
+        <v>142.649994</v>
       </c>
       <c r="G14">
         <v>62128300</v>
       </c>
       <c r="H14">
-        <v>142.64999399999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
+        <v>142.649994</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B15" s="2">
         <v>44904</v>
       </c>
       <c r="C15">
-        <v>142.33999600000001</v>
+        <v>142.339996</v>
       </c>
       <c r="D15">
         <v>145.570007</v>
       </c>
       <c r="E15">
-        <v>140.89999399999999</v>
+        <v>140.899994</v>
       </c>
       <c r="F15">
-        <v>142.16000399999999</v>
+        <v>142.160004</v>
       </c>
       <c r="G15">
         <v>76097000</v>
       </c>
       <c r="H15">
-        <v>142.16000399999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>8</v>
+        <v>142.160004</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B16" s="2">
         <v>44907</v>
@@ -867,7 +814,7 @@
         <v>144.5</v>
       </c>
       <c r="E16">
-        <v>141.05999800000001</v>
+        <v>141.059998</v>
       </c>
       <c r="F16">
         <v>144.490005</v>
@@ -879,9 +826,11 @@
         <v>144.490005</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B17" s="2">
         <v>44908</v>
@@ -905,41 +854,45 @@
         <v>145.470001</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B18" s="2">
         <v>44909</v>
       </c>
       <c r="C18">
-        <v>145.35000600000001</v>
+        <v>145.350006</v>
       </c>
       <c r="D18">
-        <v>146.66000399999999</v>
+        <v>146.660004</v>
       </c>
       <c r="E18">
-        <v>141.16000399999999</v>
+        <v>141.160004</v>
       </c>
       <c r="F18">
-        <v>143.21000699999999</v>
+        <v>143.210007</v>
       </c>
       <c r="G18">
         <v>82291200</v>
       </c>
       <c r="H18">
-        <v>143.21000699999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
+        <v>143.210007</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B19" s="2">
         <v>44910</v>
       </c>
       <c r="C19">
-        <v>141.11000100000001</v>
+        <v>141.110001</v>
       </c>
       <c r="D19">
         <v>141.800003</v>
@@ -957,18 +910,20 @@
         <v>136.5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B20" s="2">
         <v>44911</v>
       </c>
       <c r="C20">
-        <v>136.69000199999999</v>
+        <v>136.690002</v>
       </c>
       <c r="D20">
-        <v>137.64999399999999</v>
+        <v>137.649994</v>
       </c>
       <c r="E20">
         <v>133.729996</v>
@@ -983,15 +938,17 @@
         <v>134.509995</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>8</v>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B21" s="2">
         <v>44914</v>
       </c>
       <c r="C21">
-        <v>135.11000100000001</v>
+        <v>135.110001</v>
       </c>
       <c r="D21">
         <v>135.199997</v>
@@ -1000,30 +957,32 @@
         <v>131.320007</v>
       </c>
       <c r="F21">
-        <v>132.36999499999999</v>
+        <v>132.369995</v>
       </c>
       <c r="G21">
         <v>79592600</v>
       </c>
       <c r="H21">
-        <v>132.36999499999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>8</v>
+        <v>132.369995</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B22" s="2">
         <v>44915</v>
       </c>
       <c r="C22">
-        <v>131.38999899999999</v>
+        <v>131.389999</v>
       </c>
       <c r="D22">
         <v>133.25</v>
       </c>
       <c r="E22">
-        <v>129.88999899999999</v>
+        <v>129.889999</v>
       </c>
       <c r="F22">
         <v>132.300003</v>
@@ -1035,9 +994,11 @@
         <v>132.300003</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>8</v>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B23" s="2">
         <v>44916</v>
@@ -1046,7 +1007,7 @@
         <v>132.979996</v>
       </c>
       <c r="D23">
-        <v>136.80999800000001</v>
+        <v>136.809998</v>
       </c>
       <c r="E23">
         <v>132.75</v>
@@ -1061,18 +1022,20 @@
         <v>135.449997</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>8</v>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B24" s="2">
         <v>44917</v>
       </c>
       <c r="C24">
-        <v>134.35000600000001</v>
+        <v>134.350006</v>
       </c>
       <c r="D24">
-        <v>134.55999800000001</v>
+        <v>134.559998</v>
       </c>
       <c r="E24">
         <v>130.300003</v>
@@ -1087,44 +1050,48 @@
         <v>132.229996</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>8</v>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B25" s="2">
         <v>44918</v>
       </c>
       <c r="C25">
-        <v>130.91999799999999</v>
+        <v>130.919998</v>
       </c>
       <c r="D25">
-        <v>132.41999799999999</v>
+        <v>132.419998</v>
       </c>
       <c r="E25">
-        <v>129.63999899999999</v>
+        <v>129.639999</v>
       </c>
       <c r="F25">
-        <v>131.86000100000001</v>
+        <v>131.860001</v>
       </c>
       <c r="G25">
         <v>63814900</v>
       </c>
       <c r="H25">
-        <v>131.86000100000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>8</v>
+        <v>131.860001</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B26" s="2">
         <v>44922</v>
       </c>
       <c r="C26">
-        <v>131.38000500000001</v>
+        <v>131.380005</v>
       </c>
       <c r="D26">
-        <v>131.41000399999999</v>
+        <v>131.410004</v>
       </c>
       <c r="E26">
         <v>128.720001</v>
@@ -1139,15 +1106,17 @@
         <v>130.029999</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>8</v>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B27" s="2">
         <v>44923</v>
       </c>
       <c r="C27">
-        <v>129.66999799999999</v>
+        <v>129.669998</v>
       </c>
       <c r="D27">
         <v>131.029999</v>
@@ -1165,9 +1134,11 @@
         <v>126.040001</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>8</v>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B28" s="2">
         <v>44924</v>
@@ -1182,24 +1153,26 @@
         <v>127.730003</v>
       </c>
       <c r="F28">
-        <v>129.61000100000001</v>
+        <v>129.610001</v>
       </c>
       <c r="G28">
         <v>75703700</v>
       </c>
       <c r="H28">
-        <v>129.61000100000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>8</v>
+        <v>129.610001</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B29" s="2">
         <v>44925</v>
       </c>
       <c r="C29">
-        <v>128.41000399999999</v>
+        <v>128.410004</v>
       </c>
       <c r="D29">
         <v>129.949997</v>
@@ -1217,9 +1190,11 @@
         <v>129.929993</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>8</v>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B30" s="2">
         <v>44929</v>
@@ -1228,10 +1203,10 @@
         <v>130.279999</v>
       </c>
       <c r="D30">
-        <v>130.89999399999999</v>
+        <v>130.899994</v>
       </c>
       <c r="E30">
-        <v>124.16999800000001</v>
+        <v>124.169998</v>
       </c>
       <c r="F30">
         <v>125.07</v>
@@ -1243,9 +1218,11 @@
         <v>125.07</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>8</v>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B31" s="2">
         <v>44930</v>
@@ -1254,10 +1231,10 @@
         <v>126.889999</v>
       </c>
       <c r="D31">
-        <v>128.66000399999999</v>
+        <v>128.660004</v>
       </c>
       <c r="E31">
-        <v>125.08000199999999</v>
+        <v>125.080002</v>
       </c>
       <c r="F31">
         <v>126.360001</v>
@@ -1269,9 +1246,11 @@
         <v>126.360001</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>8</v>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B32" s="2">
         <v>44931</v>
@@ -1295,9 +1274,11 @@
         <v>125.019997</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>8</v>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B33" s="2">
         <v>44932</v>
@@ -1306,24 +1287,26 @@
         <v>126.010002</v>
       </c>
       <c r="D33">
-        <v>130.28999300000001</v>
+        <v>130.289993</v>
       </c>
       <c r="E33">
         <v>124.889999</v>
       </c>
       <c r="F33">
-        <v>129.61999499999999</v>
+        <v>129.619995</v>
       </c>
       <c r="G33">
         <v>87686600</v>
       </c>
       <c r="H33">
-        <v>129.61999499999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>8</v>
+        <v>129.619995</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B34" s="2">
         <v>44935</v>
@@ -1332,24 +1315,26 @@
         <v>130.470001</v>
       </c>
       <c r="D34">
-        <v>133.41000399999999</v>
+        <v>133.410004</v>
       </c>
       <c r="E34">
-        <v>129.88999899999999</v>
+        <v>129.889999</v>
       </c>
       <c r="F34">
-        <v>130.14999399999999</v>
+        <v>130.149994</v>
       </c>
       <c r="G34">
         <v>70790800</v>
       </c>
       <c r="H34">
-        <v>130.14999399999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>8</v>
+        <v>130.149994</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B35" s="2">
         <v>44936</v>
@@ -1361,7 +1346,7 @@
         <v>131.259995</v>
       </c>
       <c r="E35">
-        <v>128.11999499999999</v>
+        <v>128.119995</v>
       </c>
       <c r="F35">
         <v>130.729996</v>
@@ -1373,9 +1358,11 @@
         <v>130.729996</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>8</v>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B36" s="2">
         <v>44937</v>
@@ -1387,7 +1374,7 @@
         <v>133.509995</v>
       </c>
       <c r="E36">
-        <v>130.46000699999999</v>
+        <v>130.460007</v>
       </c>
       <c r="F36">
         <v>133.490005</v>
@@ -1399,35 +1386,39 @@
         <v>133.490005</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>8</v>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B37" s="2">
         <v>44938</v>
       </c>
       <c r="C37">
-        <v>133.88000500000001</v>
+        <v>133.880005</v>
       </c>
       <c r="D37">
         <v>134.259995</v>
       </c>
       <c r="E37">
-        <v>131.44000199999999</v>
+        <v>131.440002</v>
       </c>
       <c r="F37">
-        <v>133.41000399999999</v>
+        <v>133.410004</v>
       </c>
       <c r="G37">
         <v>71379600</v>
       </c>
       <c r="H37">
-        <v>133.41000399999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>8</v>
+        <v>133.410004</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B38" s="2">
         <v>44939</v>
@@ -1436,10 +1427,10 @@
         <v>132.029999</v>
       </c>
       <c r="D38">
-        <v>134.91999799999999</v>
+        <v>134.919998</v>
       </c>
       <c r="E38">
-        <v>131.66000399999999</v>
+        <v>131.660004</v>
       </c>
       <c r="F38">
         <v>134.759995</v>
@@ -1451,35 +1442,39 @@
         <v>134.759995</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>8</v>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B39" s="2">
         <v>44943</v>
       </c>
       <c r="C39">
-        <v>134.83000200000001</v>
+        <v>134.830002</v>
       </c>
       <c r="D39">
-        <v>137.28999300000001</v>
+        <v>137.289993</v>
       </c>
       <c r="E39">
-        <v>134.13000500000001</v>
+        <v>134.130005</v>
       </c>
       <c r="F39">
-        <v>135.94000199999999</v>
+        <v>135.940002</v>
       </c>
       <c r="G39">
         <v>63646600</v>
       </c>
       <c r="H39">
-        <v>135.94000199999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>8</v>
+        <v>135.940002</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="B40" s="2">
         <v>44944</v>
@@ -1488,19 +1483,19 @@
         <v>136.820007</v>
       </c>
       <c r="D40">
-        <v>138.61000100000001</v>
+        <v>138.610001</v>
       </c>
       <c r="E40">
         <v>135.029999</v>
       </c>
       <c r="F40">
-        <v>135.21000699999999</v>
+        <v>135.210007</v>
       </c>
       <c r="G40">
         <v>69567000</v>
       </c>
       <c r="H40">
-        <v>135.21000699999999</v>
+        <v>135.210007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a read from excel chunk - pricing from a list of tickers has to be added.
</commit_message>
<xml_diff>
--- a/aapl.xlsx
+++ b/aapl.xlsx
@@ -1,24 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/286054357d240948/Github/Intro to Finance/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_EFF9FFC08F79A89360642C52EA7BD272EA43B8E4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AD00668-FFAE-45D5-B05C-3BBA91EB435D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-26970" yWindow="1635" windowWidth="24270" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="9">
+  <si>
+    <t>symbol</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>adjusted</t>
+  </si>
+  <si>
+    <t>AAPL</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd HH:mm:ss UTC"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss\ \U\T\C"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +118,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -113,7 +172,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -145,9 +204,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,6 +256,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -354,72 +449,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>symbol</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>open</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>high</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>low</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>close</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>volume</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>adjusted</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>44886</v>
       </c>
       <c r="C2">
-        <v>150.160004</v>
+        <v>150.16000399999999</v>
       </c>
       <c r="D2">
-        <v>150.369995</v>
+        <v>150.36999499999999</v>
       </c>
       <c r="E2">
         <v>147.720001</v>
@@ -434,20 +513,18 @@
         <v>148.009995</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>44887</v>
       </c>
       <c r="C3">
-        <v>148.130005</v>
+        <v>148.13000500000001</v>
       </c>
       <c r="D3">
-        <v>150.419998</v>
+        <v>150.41999799999999</v>
       </c>
       <c r="E3">
         <v>146.929993</v>
@@ -462,11 +539,9 @@
         <v>150.179993</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>44888</v>
@@ -475,10 +550,10 @@
         <v>149.449997</v>
       </c>
       <c r="D4">
-        <v>151.830002</v>
+        <v>151.83000200000001</v>
       </c>
       <c r="E4">
-        <v>149.339996</v>
+        <v>149.33999600000001</v>
       </c>
       <c r="F4">
         <v>151.070007</v>
@@ -490,51 +565,47 @@
         <v>151.070007</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>44890</v>
       </c>
       <c r="C5">
-        <v>148.309998</v>
+        <v>148.30999800000001</v>
       </c>
       <c r="D5">
-        <v>148.880005</v>
+        <v>148.88000500000001</v>
       </c>
       <c r="E5">
-        <v>147.119995</v>
+        <v>147.11999499999999</v>
       </c>
       <c r="F5">
-        <v>148.110001</v>
+        <v>148.11000100000001</v>
       </c>
       <c r="G5">
         <v>35195900</v>
       </c>
       <c r="H5">
-        <v>148.110001</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>148.11000100000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>44893</v>
       </c>
       <c r="C6">
-        <v>145.139999</v>
+        <v>145.13999899999999</v>
       </c>
       <c r="D6">
-        <v>146.639999</v>
+        <v>146.63999899999999</v>
       </c>
       <c r="E6">
-        <v>143.380005</v>
+        <v>143.38000500000001</v>
       </c>
       <c r="F6">
         <v>144.220001</v>
@@ -546,45 +617,41 @@
         <v>144.220001</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>44894</v>
       </c>
       <c r="C7">
-        <v>144.289993</v>
+        <v>144.28999300000001</v>
       </c>
       <c r="D7">
-        <v>144.809998</v>
+        <v>144.80999800000001</v>
       </c>
       <c r="E7">
-        <v>140.350006</v>
+        <v>140.35000600000001</v>
       </c>
       <c r="F7">
-        <v>141.169998</v>
+        <v>141.16999799999999</v>
       </c>
       <c r="G7">
         <v>83763800</v>
       </c>
       <c r="H7">
-        <v>141.169998</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>141.16999799999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>44895</v>
       </c>
       <c r="C8">
-        <v>141.399994</v>
+        <v>141.39999399999999</v>
       </c>
       <c r="D8">
         <v>148.720001</v>
@@ -602,67 +669,61 @@
         <v>148.029999</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
       </c>
       <c r="B9" s="2">
         <v>44896</v>
       </c>
       <c r="C9">
-        <v>148.210007</v>
+        <v>148.21000699999999</v>
       </c>
       <c r="D9">
-        <v>149.130005</v>
+        <v>149.13000500000001</v>
       </c>
       <c r="E9">
-        <v>146.610001</v>
+        <v>146.61000100000001</v>
       </c>
       <c r="F9">
-        <v>148.309998</v>
+        <v>148.30999800000001</v>
       </c>
       <c r="G9">
         <v>71250400</v>
       </c>
       <c r="H9">
-        <v>148.309998</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>148.30999800000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>44897</v>
       </c>
       <c r="C10">
-        <v>145.960007</v>
+        <v>145.96000699999999</v>
       </c>
       <c r="D10">
         <v>148</v>
       </c>
       <c r="E10">
-        <v>145.649994</v>
+        <v>145.64999399999999</v>
       </c>
       <c r="F10">
-        <v>147.809998</v>
+        <v>147.80999800000001</v>
       </c>
       <c r="G10">
         <v>65447400</v>
       </c>
       <c r="H10">
-        <v>147.809998</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>147.80999800000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
       </c>
       <c r="B11" s="2">
         <v>44900</v>
@@ -671,26 +732,24 @@
         <v>147.770004</v>
       </c>
       <c r="D11">
-        <v>150.919998</v>
+        <v>150.91999799999999</v>
       </c>
       <c r="E11">
         <v>145.770004</v>
       </c>
       <c r="F11">
-        <v>146.630005</v>
+        <v>146.63000500000001</v>
       </c>
       <c r="G11">
         <v>68826400</v>
       </c>
       <c r="H11">
-        <v>146.630005</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>146.63000500000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
       </c>
       <c r="B12" s="2">
         <v>44901</v>
@@ -702,107 +761,99 @@
         <v>147.300003</v>
       </c>
       <c r="E12">
-        <v>141.919998</v>
+        <v>141.91999799999999</v>
       </c>
       <c r="F12">
-        <v>142.910004</v>
+        <v>142.91000399999999</v>
       </c>
       <c r="G12">
         <v>64727200</v>
       </c>
       <c r="H12">
-        <v>142.910004</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>142.91000399999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>44902</v>
       </c>
       <c r="C13">
-        <v>142.190002</v>
+        <v>142.19000199999999</v>
       </c>
       <c r="D13">
-        <v>143.369995</v>
+        <v>143.36999499999999</v>
       </c>
       <c r="E13">
         <v>140</v>
       </c>
       <c r="F13">
-        <v>140.940002</v>
+        <v>140.94000199999999</v>
       </c>
       <c r="G13">
         <v>69721100</v>
       </c>
       <c r="H13">
-        <v>140.940002</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>140.94000199999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
       </c>
       <c r="B14" s="2">
         <v>44903</v>
       </c>
       <c r="C14">
-        <v>142.360001</v>
+        <v>142.36000100000001</v>
       </c>
       <c r="D14">
         <v>143.520004</v>
       </c>
       <c r="E14">
-        <v>141.100006</v>
+        <v>141.10000600000001</v>
       </c>
       <c r="F14">
-        <v>142.649994</v>
+        <v>142.64999399999999</v>
       </c>
       <c r="G14">
         <v>62128300</v>
       </c>
       <c r="H14">
-        <v>142.649994</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>142.64999399999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
       </c>
       <c r="B15" s="2">
         <v>44904</v>
       </c>
       <c r="C15">
-        <v>142.339996</v>
+        <v>142.33999600000001</v>
       </c>
       <c r="D15">
         <v>145.570007</v>
       </c>
       <c r="E15">
-        <v>140.899994</v>
+        <v>140.89999399999999</v>
       </c>
       <c r="F15">
-        <v>142.160004</v>
+        <v>142.16000399999999</v>
       </c>
       <c r="G15">
         <v>76097000</v>
       </c>
       <c r="H15">
-        <v>142.160004</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>142.16000399999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
       </c>
       <c r="B16" s="2">
         <v>44907</v>
@@ -814,7 +865,7 @@
         <v>144.5</v>
       </c>
       <c r="E16">
-        <v>141.059998</v>
+        <v>141.05999800000001</v>
       </c>
       <c r="F16">
         <v>144.490005</v>
@@ -826,11 +877,9 @@
         <v>144.490005</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
       </c>
       <c r="B17" s="2">
         <v>44908</v>
@@ -854,45 +903,41 @@
         <v>145.470001</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
       </c>
       <c r="B18" s="2">
         <v>44909</v>
       </c>
       <c r="C18">
-        <v>145.350006</v>
+        <v>145.35000600000001</v>
       </c>
       <c r="D18">
-        <v>146.660004</v>
+        <v>146.66000399999999</v>
       </c>
       <c r="E18">
-        <v>141.160004</v>
+        <v>141.16000399999999</v>
       </c>
       <c r="F18">
-        <v>143.210007</v>
+        <v>143.21000699999999</v>
       </c>
       <c r="G18">
         <v>82291200</v>
       </c>
       <c r="H18">
-        <v>143.210007</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>143.21000699999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
       </c>
       <c r="B19" s="2">
         <v>44910</v>
       </c>
       <c r="C19">
-        <v>141.110001</v>
+        <v>141.11000100000001</v>
       </c>
       <c r="D19">
         <v>141.800003</v>
@@ -910,20 +955,18 @@
         <v>136.5</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
       </c>
       <c r="B20" s="2">
         <v>44911</v>
       </c>
       <c r="C20">
-        <v>136.690002</v>
+        <v>136.69000199999999</v>
       </c>
       <c r="D20">
-        <v>137.649994</v>
+        <v>137.64999399999999</v>
       </c>
       <c r="E20">
         <v>133.729996</v>
@@ -938,17 +981,15 @@
         <v>134.509995</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>8</v>
       </c>
       <c r="B21" s="2">
         <v>44914</v>
       </c>
       <c r="C21">
-        <v>135.110001</v>
+        <v>135.11000100000001</v>
       </c>
       <c r="D21">
         <v>135.199997</v>
@@ -957,32 +998,30 @@
         <v>131.320007</v>
       </c>
       <c r="F21">
-        <v>132.369995</v>
+        <v>132.36999499999999</v>
       </c>
       <c r="G21">
         <v>79592600</v>
       </c>
       <c r="H21">
-        <v>132.369995</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>132.36999499999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>8</v>
       </c>
       <c r="B22" s="2">
         <v>44915</v>
       </c>
       <c r="C22">
-        <v>131.389999</v>
+        <v>131.38999899999999</v>
       </c>
       <c r="D22">
         <v>133.25</v>
       </c>
       <c r="E22">
-        <v>129.889999</v>
+        <v>129.88999899999999</v>
       </c>
       <c r="F22">
         <v>132.300003</v>
@@ -994,11 +1033,9 @@
         <v>132.300003</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
       </c>
       <c r="B23" s="2">
         <v>44916</v>
@@ -1007,7 +1044,7 @@
         <v>132.979996</v>
       </c>
       <c r="D23">
-        <v>136.809998</v>
+        <v>136.80999800000001</v>
       </c>
       <c r="E23">
         <v>132.75</v>
@@ -1022,20 +1059,18 @@
         <v>135.449997</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
       </c>
       <c r="B24" s="2">
         <v>44917</v>
       </c>
       <c r="C24">
-        <v>134.350006</v>
+        <v>134.35000600000001</v>
       </c>
       <c r="D24">
-        <v>134.559998</v>
+        <v>134.55999800000001</v>
       </c>
       <c r="E24">
         <v>130.300003</v>
@@ -1050,48 +1085,44 @@
         <v>132.229996</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>8</v>
       </c>
       <c r="B25" s="2">
         <v>44918</v>
       </c>
       <c r="C25">
-        <v>130.919998</v>
+        <v>130.91999799999999</v>
       </c>
       <c r="D25">
-        <v>132.419998</v>
+        <v>132.41999799999999</v>
       </c>
       <c r="E25">
-        <v>129.639999</v>
+        <v>129.63999899999999</v>
       </c>
       <c r="F25">
-        <v>131.860001</v>
+        <v>131.86000100000001</v>
       </c>
       <c r="G25">
         <v>63814900</v>
       </c>
       <c r="H25">
-        <v>131.860001</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>131.86000100000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>8</v>
       </c>
       <c r="B26" s="2">
         <v>44922</v>
       </c>
       <c r="C26">
-        <v>131.380005</v>
+        <v>131.38000500000001</v>
       </c>
       <c r="D26">
-        <v>131.410004</v>
+        <v>131.41000399999999</v>
       </c>
       <c r="E26">
         <v>128.720001</v>
@@ -1106,17 +1137,15 @@
         <v>130.029999</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
       </c>
       <c r="B27" s="2">
         <v>44923</v>
       </c>
       <c r="C27">
-        <v>129.669998</v>
+        <v>129.66999799999999</v>
       </c>
       <c r="D27">
         <v>131.029999</v>
@@ -1134,11 +1163,9 @@
         <v>126.040001</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>8</v>
       </c>
       <c r="B28" s="2">
         <v>44924</v>
@@ -1153,26 +1180,24 @@
         <v>127.730003</v>
       </c>
       <c r="F28">
-        <v>129.610001</v>
+        <v>129.61000100000001</v>
       </c>
       <c r="G28">
         <v>75703700</v>
       </c>
       <c r="H28">
-        <v>129.610001</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>129.61000100000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>8</v>
       </c>
       <c r="B29" s="2">
         <v>44925</v>
       </c>
       <c r="C29">
-        <v>128.410004</v>
+        <v>128.41000399999999</v>
       </c>
       <c r="D29">
         <v>129.949997</v>
@@ -1190,11 +1215,9 @@
         <v>129.929993</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>8</v>
       </c>
       <c r="B30" s="2">
         <v>44929</v>
@@ -1203,10 +1226,10 @@
         <v>130.279999</v>
       </c>
       <c r="D30">
-        <v>130.899994</v>
+        <v>130.89999399999999</v>
       </c>
       <c r="E30">
-        <v>124.169998</v>
+        <v>124.16999800000001</v>
       </c>
       <c r="F30">
         <v>125.07</v>
@@ -1218,11 +1241,9 @@
         <v>125.07</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>8</v>
       </c>
       <c r="B31" s="2">
         <v>44930</v>
@@ -1231,10 +1252,10 @@
         <v>126.889999</v>
       </c>
       <c r="D31">
-        <v>128.660004</v>
+        <v>128.66000399999999</v>
       </c>
       <c r="E31">
-        <v>125.080002</v>
+        <v>125.08000199999999</v>
       </c>
       <c r="F31">
         <v>126.360001</v>
@@ -1246,11 +1267,9 @@
         <v>126.360001</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>8</v>
       </c>
       <c r="B32" s="2">
         <v>44931</v>
@@ -1274,11 +1293,9 @@
         <v>125.019997</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>8</v>
       </c>
       <c r="B33" s="2">
         <v>44932</v>
@@ -1287,26 +1304,24 @@
         <v>126.010002</v>
       </c>
       <c r="D33">
-        <v>130.289993</v>
+        <v>130.28999300000001</v>
       </c>
       <c r="E33">
         <v>124.889999</v>
       </c>
       <c r="F33">
-        <v>129.619995</v>
+        <v>129.61999499999999</v>
       </c>
       <c r="G33">
         <v>87686600</v>
       </c>
       <c r="H33">
-        <v>129.619995</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>129.61999499999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>8</v>
       </c>
       <c r="B34" s="2">
         <v>44935</v>
@@ -1315,26 +1330,24 @@
         <v>130.470001</v>
       </c>
       <c r="D34">
-        <v>133.410004</v>
+        <v>133.41000399999999</v>
       </c>
       <c r="E34">
-        <v>129.889999</v>
+        <v>129.88999899999999</v>
       </c>
       <c r="F34">
-        <v>130.149994</v>
+        <v>130.14999399999999</v>
       </c>
       <c r="G34">
         <v>70790800</v>
       </c>
       <c r="H34">
-        <v>130.149994</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>130.14999399999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>8</v>
       </c>
       <c r="B35" s="2">
         <v>44936</v>
@@ -1346,7 +1359,7 @@
         <v>131.259995</v>
       </c>
       <c r="E35">
-        <v>128.119995</v>
+        <v>128.11999499999999</v>
       </c>
       <c r="F35">
         <v>130.729996</v>
@@ -1358,11 +1371,9 @@
         <v>130.729996</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>8</v>
       </c>
       <c r="B36" s="2">
         <v>44937</v>
@@ -1374,7 +1385,7 @@
         <v>133.509995</v>
       </c>
       <c r="E36">
-        <v>130.460007</v>
+        <v>130.46000699999999</v>
       </c>
       <c r="F36">
         <v>133.490005</v>
@@ -1386,39 +1397,35 @@
         <v>133.490005</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>8</v>
       </c>
       <c r="B37" s="2">
         <v>44938</v>
       </c>
       <c r="C37">
-        <v>133.880005</v>
+        <v>133.88000500000001</v>
       </c>
       <c r="D37">
         <v>134.259995</v>
       </c>
       <c r="E37">
-        <v>131.440002</v>
+        <v>131.44000199999999</v>
       </c>
       <c r="F37">
-        <v>133.410004</v>
+        <v>133.41000399999999</v>
       </c>
       <c r="G37">
         <v>71379600</v>
       </c>
       <c r="H37">
-        <v>133.410004</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>133.41000399999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>8</v>
       </c>
       <c r="B38" s="2">
         <v>44939</v>
@@ -1427,10 +1434,10 @@
         <v>132.029999</v>
       </c>
       <c r="D38">
-        <v>134.919998</v>
+        <v>134.91999799999999</v>
       </c>
       <c r="E38">
-        <v>131.660004</v>
+        <v>131.66000399999999</v>
       </c>
       <c r="F38">
         <v>134.759995</v>
@@ -1442,39 +1449,35 @@
         <v>134.759995</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>8</v>
       </c>
       <c r="B39" s="2">
         <v>44943</v>
       </c>
       <c r="C39">
-        <v>134.830002</v>
+        <v>134.83000200000001</v>
       </c>
       <c r="D39">
-        <v>137.289993</v>
+        <v>137.28999300000001</v>
       </c>
       <c r="E39">
-        <v>134.130005</v>
+        <v>134.13000500000001</v>
       </c>
       <c r="F39">
-        <v>135.940002</v>
+        <v>135.94000199999999</v>
       </c>
       <c r="G39">
         <v>63646600</v>
       </c>
       <c r="H39">
-        <v>135.940002</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
+        <v>135.94000199999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>8</v>
       </c>
       <c r="B40" s="2">
         <v>44944</v>
@@ -1483,19 +1486,19 @@
         <v>136.820007</v>
       </c>
       <c r="D40">
-        <v>138.610001</v>
+        <v>138.61000100000001</v>
       </c>
       <c r="E40">
         <v>135.029999</v>
       </c>
       <c r="F40">
-        <v>135.210007</v>
+        <v>135.21000699999999</v>
       </c>
       <c r="G40">
         <v>69567000</v>
       </c>
       <c r="H40">
-        <v>135.210007</v>
+        <v>135.21000699999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>